<commit_message>
Update a lot of things
</commit_message>
<xml_diff>
--- a/Documentation/Mission 3/Matrice RACI.xlsx
+++ b/Documentation/Mission 3/Matrice RACI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\Cours\Projet Annuel\Projet-Annuel-BOURMIER-Jordan-ROUVILLE-Quentin-Groupe-1\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\Cours\Projet Annuel\Projet-Annuel-BOURMIER-Jordan-ROUVILLE-Quentin-Groupe-1\Documentation\Mission 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB47297A-F30F-42BA-8C05-99048E20512D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E021BF-3EE6-4D94-8A96-1F7356D6A3C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12825" yWindow="0" windowWidth="15975" windowHeight="16200" xr2:uid="{4C5EBE2D-C22E-4A8E-A84F-E76903108394}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4C5EBE2D-C22E-4A8E-A84F-E76903108394}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>BOURMIER Jordan</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Légende :</t>
   </si>
   <si>
-    <t>A :</t>
-  </si>
-  <si>
     <t xml:space="preserve">C : </t>
   </si>
   <si>
@@ -79,6 +76,30 @@
   </si>
   <si>
     <t>AC</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Prestataire</t>
+  </si>
+  <si>
+    <t>R :</t>
+  </si>
+  <si>
+    <t>I :</t>
+  </si>
+  <si>
+    <t>Seconde main</t>
+  </si>
+  <si>
+    <t>Aller une troisième si elle veut au moins elle est au courant</t>
+  </si>
+  <si>
+    <t>Consulter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Au moins un A :</t>
   </si>
 </sst>
 </file>
@@ -114,10 +135,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,101 +457,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B34D8C9-8180-42E7-AA01-2CFDD4A95DD5}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="3" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="1"/>
-    <col min="6" max="6" width="111.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="2"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>